<commit_message>
refatoração da CPU - SLL não funciona
</commit_message>
<xml_diff>
--- a/Simulador de Computador RISC-V/tabela de operações.xlsx
+++ b/Simulador de Computador RISC-V/tabela de operações.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migue\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migue\source\repos\Simulador de Computador RISC-V\Simulador de Computador RISC-V\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB497975-DED3-4D45-B068-2731594512CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15551558-ED6A-4551-BC01-15BA9A5D49CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3CEE4B17-4345-4B21-9184-5A5D1297C154}"/>
   </bookViews>
@@ -1021,7 +1021,7 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>